<commit_message>
config now takes constant regions
</commit_message>
<xml_diff>
--- a/blastdb/sampled_residues.xlsx
+++ b/blastdb/sampled_residues.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>MHC A3 W242</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>MHC A3 G246</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -524,6 +529,11 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>WT</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>GT</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Writes complete sequences to extracted file
</commit_message>
<xml_diff>
--- a/blastdb/sampled_residues.xlsx
+++ b/blastdb/sampled_residues.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>MHC A3 W242</t>
+          <t>B2M W242</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>MHC A3 G246</t>
+          <t>B2M G246</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Can now write to ranked file when multiple proteins are extracted
</commit_message>
<xml_diff>
--- a/blastdb/sampled_residues.xlsx
+++ b/blastdb/sampled_residues.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,16 +474,6 @@
           <t>MHC A3 V234</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>B2M W242</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>B2M G246</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -524,16 +514,6 @@
       <c r="H2" t="inlineStr">
         <is>
           <t>VN</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>GT</t>
         </is>
       </c>
     </row>

</xml_diff>